<commit_message>
fixed error with reflecting on the prompt instead of the reflections
Fixed bug. Issue was with the input dataset, some client statements recorded as prompts and responses were from the therapist
</commit_message>
<xml_diff>
--- a/example_results.xlsx
+++ b/example_results.xlsx
@@ -473,17 +473,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>well she got really angry at me because on the way to my room my idiot sister got in the way so I pushed her out of the way she's just annoying so then I went into my room the only place that I really feel safe slammed the door and then mums favorite picture fell on the floor</t>
+          <t>it's a bad experience for him</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>thank you for sharing that with me because it really and being for being so honest about your anger because what it does is help I don't know if it's helping you but it's certainly helping me to understand that this is really big for you and it's a big expression but surprisingly you know anger anger's a good thing in a way because it's it's letting you know that something wasn't right and wasn't fair that he he just did change the thing without your permission without you knowing so in some ways you had a right to be angry but what happens what I heard you saying in as you were telling me what happened next what happened next was that your anger took charge and he it did more than what it's meant to do your your anger is just just to let you know that you're angry okay but what it did what I feel it did it just pushed you out of the road and said I'm I'm taking control here so Jane when you were angry did you feel it anywhere in your body</t>
+          <t>and now he's moved out I don't have my job he's moved out you know he's got the kids he said I can't be trusted with my kids so you don't</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Response : no, nothing. It felt very different inside myself now where before maybe after an argument or whatever cause we both knew exactly why our arguments happen sometimes they go back years ago which makes sense since everyone knows each other better by their own experiences anyway its hard enough having two people who share similar interests together talking over dinner while drinking wine and eating pizza  it feels weirdly uncomfortable even worse still seeing him sitting alone watching TV again making fun jokes around his friends instead listening intently listen up please tell us anything else? ok fine thanks sorry i think im done reading yet</t>
+          <t>oh okay so if you were to move out would you still be able to work?</t>
         </is>
       </c>
     </row>
@@ -499,17 +499,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sure um as you know I'm Andrea I uh I'm a junior I'm in the marching band I played at center sacks I mean yeah I'm also in the little bit of a band geek I play you know the Wind Ensemble and the Jazz Band things like that</t>
+          <t>something else could change</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>wow you really are involved in music</t>
+          <t>yeah I don't know what</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Receptionist 1 (1): Hi, how may I assist? Thank You for coming. We would appreciate any assistance from anyone interested on helping us find someone else willing/able enough to participate. Please contact info@marijuanaforlifeusa</t>
+          <t>do you want to talk about it?</t>
         </is>
       </c>
     </row>
@@ -525,15 +525,19 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>it's overwhelming that getting all your stuff inside working out strategies</t>
+          <t>and why why do you want to lose weight</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>I think that you know girls are always overachievers and we can't just chill and like even my fans always like why don't you just relax they're plump up your deal but I'm trying to think that but I don't like it's a big deal school some things ago because I'm not really talented with my music okay dance or any of those things but so many people are into it so school is like my gift I do good and I understand it so to not feel secure and that is kind of</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>well so really recently actually my older sister has had a lot of health concerns relate to her weight and it just sort of jostled me a little bit because we're so similar</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>she's overweight?</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -547,17 +551,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>slow down and maybe stay calm and just think that think of the letter e easy whatever that that word easy would make you feel</t>
+          <t>very fun all right and how are things going in school for you</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>okay</t>
+          <t>pretty good grades have been pretty all right still like 3.7 ish</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>I've been thinking about writing something because if someone says "you can write anything" well, let's say they want to read your thoughts. You could go ahead right? So why am i saying yes please tell us some stories are great story ideas! And also try telling them things people might find interesting too which will help keep their interest level high as long time readers who may never get into reading fiction before probably aren´t interested either. But even though those two options sound pretty cool, actually most writers tend towards being very specific (like an author) while others prefer letting loose without having much detail behind each sentence   They usually start off simple enough where everyone knows exactly whats happening and once everything gets started however many words later its hard knowing whether every single thing has meaning beyond simply making sure nothing feels superfluous :P It takes longer than expected especially since sometimes authors use short sentences instead Of course after finishing first drafts often times only half-way done until final version The problem comes again</t>
+          <t>well thanks for taking time out to talk to us today</t>
         </is>
       </c>
     </row>
@@ -573,17 +577,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>no not really</t>
+          <t>mm-hmm and do you feel like that's working pretty well for you or you sometimes exceed that limit or or what do you think</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>what are you losing</t>
+          <t>for the most part it works pretty well because like I said people you know people come asking me trying to pressure me I'll be like no I'm good I have you know I still have so I'm like I'll get some later and then never end up getting anything but sometimes they'll be like hey let's take a shot and everyone's got it around like the kitchen or something ready to take a shot and then at that point I'll be like oh well maybe I can take one more and that's when I start you know falling into</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>reflected response from her friend, she said "I don´t know if we should do this or something" then they both looked at eachothers eyes as though looking into their own hearts. They didn`T say anything else until after all was over</t>
+          <t>so you just want to make sure you're taking enough?</t>
         </is>
       </c>
     </row>
@@ -599,17 +603,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>I pick up a prescription</t>
+          <t>uh-huh well why did you say six or seven rather than like a four</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>okay and what's your name</t>
+          <t>um because I still think it's it's important</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Response 2: My Name Is Michael C. Reply Delete</t>
+          <t>Okay so you know you can't smoke on the weekends, right?</t>
         </is>
       </c>
     </row>
@@ -625,17 +629,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>I think those two and um respect respect</t>
+          <t>okay so what's been going on what is gonna happen</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>okay can you tell me a little bit about why you picked those three</t>
+          <t>um well I am gonna have to go to court soon and I know that I'm probably gonna have to get some type of like treatment or something like that but I really just don't want to so I just I'm just coming here because I don't know maybe I can like get out of it if I'm getting some type of treatment but I don't know</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Response : Well first off, uh this is something where there was an article in The New York Times last week called "The Biggest Health Risk You Can Avoid" which talked specifically around diabetes. And one of the things people who read these articles said after reading them was basically 'I know someone whose life changed forever' or whatever but then also their family members say too many doctors treat diabetic patients as though somehow all diabetics should get treatment at once rather than treating each individual disease individually. So yeah obviously being diagnosed early enough before age 40 makes sense especially considering our current obesity epidemic,but now even more importantly let us talk about dieting right? Dieters tend towards eating less often (especially during periods such up-and -down cycles) while non dieter eat much higher amounts compared to other groups including vegetarians/vegans   This means most diets fail due mainly from lack o f nutrients available through food intake alone without any help by dietary changes resulting either via exercise training etc</t>
+          <t>ok so how long will it take?</t>
         </is>
       </c>
     </row>
@@ -651,15 +655,19 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>right I was trying not to do all those things so I thought you know it to stop I just have to it kind of took me over I took it changed my focus and I had that to focus on so I didn't actually stop in the middle the highway but I you know</t>
+          <t>well if you don't mind John if we can go over to the side area and I can discuss with you further kind of see your ankle John</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>I am so proud of you that is awesome Taylor think I am just that couldn't be happier and wait till we tell the group</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>sure</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>okay cool thanks man</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -673,17 +681,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>I think it's good because my sugars aren't about 14 every day so it must be working it must work her maybe even a couple of days so it's pretty effective</t>
+          <t>yeah so your financial stress may be increased by the fact that you're drinking</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>do you feel like you've seen some real improvements on that</t>
+          <t>yeah kind of defeating the purpose there</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reflections : yeah, definitely. It feels great being able get back onto track again after such long periods where sugar levels weren´t high enough or too low which means less energy intake overall So thanks guys!</t>
+          <t>but you've got to do something about it right?</t>
         </is>
       </c>
     </row>
@@ -699,15 +707,19 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>well I have some ideas on that if you'd be open to hearing them</t>
+          <t>huh okay so on the one side some of the fun things associated with alcohol are people are just more relaxed sort of carefree and kind of let loose a little bit more on the other hand there's a little bit more I guess planning involved because you have to make sure that you're doing it safely or as safe as you can and then there can be some other consequences like throwing up or even if it's not you that sometimes you're stuck your your fun is sort of ruined when you're stuck dealing with a friend you drink too much okay any other not-so-good things about the alcohol</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>sure</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>yeah people can get a little like sloppy I guess like they're all loose like with people and corners doing things that should be done in private and that kind of stuff</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>oh wow that's interesting</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -721,17 +733,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>so you're stuck there</t>
+          <t>like forget about problems</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>yeah it kind of like I would like realized that like drinking and using marijuana hasn't like got me anywhere positive really but it's like the only thing that like I know I just that's all I do usually and it's all in that mix we ever like feel better</t>
+          <t>yeah</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reflecting: what about alcohol? What does pot affect for someone trying new drugs or doing them on their own. Is weed an addiction, if yes how long has cannabis been around as opposed Alcohol use being addictive? How many times per day will smoking cigarettes cause problems when compared Cannabis usage causing no problem whatsoever. Do these two substances lead into each others' addictions,what effect both may bring upon those addicted individuals</t>
+          <t>well let's talk about this problem</t>
         </is>
       </c>
     </row>
@@ -747,17 +759,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>now what side effects did your doctor tell you that this medication made cause</t>
+          <t>I want you have a seat here sure so to start off I'm just going to verify your information real quick so we said your name's Larry seedorf is your date of birth let's see</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>I don't know I mean he you know he did say that hopefully would be better for my my legs right</t>
+          <t>129 68 okay</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reflects : how long has she said no? What does her opinion look from here? Is everything good yet, well we haven´t seen them before. So why didn` t anyone see him earlier,what happened after his surgery. Did someone call 911 first thing last night (or later)   and ask questions during their interview process which may explain away certain details such As who called whom etc.? How many times will police officers check IDs prior/after seeing witnesses; whether witness identification cards show names listed by name only ; If officer asks person "What type"of license plate number(if applicable); Does Officer need ID card showing driver�name &amp; date of birth - Driver must provide photo proof including passport size photograph / driving record photos.; Do Police Officers require drivers' licenses issued outside US without expiration dates printed prominently above windshield wiper blades.(If available). Are Drivers required fingerprinted upon arrival into city limits area – No! The City cannot deny entry based solely off fingerprints alone</t>
+          <t>oh wow that's pretty cool</t>
         </is>
       </c>
     </row>
@@ -773,17 +785,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>I'd say about like like a six or a seven oh I like to work on it but you know if I get around to it I get around to if I don't I don't</t>
+          <t>yeah I understand it does sound like you're worried about getting holes in your teeth though there are a few options that you can do to help improve how you consume sugar would you like to hear about those</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>uh-huh well why did you say six or seven rather than like a four</t>
+          <t>well I don't like getting feelings so that would be great</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reflecting again, how do we talk through these issues? What are our options for dealing effectively without resortating into violence. How does one deal constructively while still being able/willing enough to engage others as they need us most? And then finally where should someone go from here after having been arrested because their actions have caused harm (or at least hurt) other individuals. If anyone has any thoughts please share them below!</t>
+          <t>oh ok cool so if you were going to try one thing, what would it be?</t>
         </is>
       </c>
     </row>
@@ -799,17 +811,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>that's what really only leaves me at five or six</t>
+          <t>oh nice</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>okay so what can we do to get you at say like a nine or ten level of confidence</t>
+          <t>I'm a big boy</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>I don't even remember how many times i got up from bed when people were talking on their cell phones, then again sometimes things are hard for us as parents especially since kids tend towards being shy. So let alone trying new activities which means doing them every night before school starts? It seems impossible right now! But here comes another question; What would happen without these exercises? Would everything still feel good enough,would everyone stay healthy.Would anyone actually enjoy themselves anymore! And finally ; How long will those exercise sessions last until someone gets sick (or worse) :D</t>
+          <t>so you're going to start taking care of yourself better?</t>
         </is>
       </c>
     </row>
@@ -825,17 +837,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>um I guess yes help me figure out whether or not like I do want to stop drinking or using drugs I mean that might be something that I have to do right now I don't really want to so I don't know if I could like get to a place where I actually do want to stop it'd be easier to actually do it then</t>
+          <t>agree with my secret</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>like a like a place in terms of your thinking like your mentality</t>
+          <t>honestly I don't know I mean I was swear I don't have a problem but how am I gonna you know my best friend will talk to me I mean she drinks more than anyone I know and she said I'm going overboard you know she tried to tell me paste want for everyone she has you know so and I don't want to tell you this but I got another DUI</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reflections : how would i say? Like for example, let us talk specifically around sex. You mentioned before on here, which seems very important especially since most women find themselves sexually attracted towards men. So does being interested by someone else affect sexual attraction? Or perhaps even vice versa depending upon gender differences between genders (like male interest may increase female desire ) What kinds/levels / levels of arousal from another person affects sexuality differently among different individuals based solely off their own individual experiences rather compared against others' experience such feelings related only toward them also seem relevant given current research findings regarding brain structure changes associated both directly through hormones involved via testosterone production [1] –[4]. In addition studies suggest increased activity throughout parts "the limbic system" including amygdala; hippocampus region implicated in emotional processing involving reward anticipation resulting primarily due either direct effects mediated indirectly thru dopamine release pathways leading to enhanced motivation &amp; pleasure seeking behavior induced mainly after exposure stimuli eliciting greater activation following stimulation cues suggesting heightened sensitivity across regions contributing to higher</t>
+          <t>oh yeah right</t>
         </is>
       </c>
     </row>
@@ -851,17 +863,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>yeah I don't know what I'm gonna do I can't imagine like not drinking and using drugs I'm sure I would like leave court that day thinking I would but I don't know what happened when I get home for the next day or that day</t>
+          <t>right you've got it okay good what questions do you have for me about this medication</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>let's go back a couple of steps how long have you been using the alcohol marijuana</t>
+          <t>I mean you know I mean I just hope that doesn't cause the pain I mean obviously you know it's frustrating I'm good not have any problems and then start taking medicine and starting to have problems</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Response 2: oh wow ok cool thanks thank you very much good morning sweetheart i hope there wasn´t anything wrong please come over tomorrow night if any problems arise from tonight, sorry no worries. Thank You!</t>
+          <t>oh ok cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool cool</t>
         </is>
       </c>
     </row>
@@ -877,17 +889,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>and what what promise you to pick a five or six</t>
+          <t>and when you use the opposites of a happening and what I want you to do is first put what preceded what that was happening before you decided to use it for this technique so whether it was an argument your mother or somebody cut you off you know you're getting stressed about a homework assignment whatever happens to be what happened before which behavior you choose to use which skill set you're going to implement and then how do you sell afterwards okay and it made you feel calmer happier got along better with your mother you were able to finish your assignment without anxiety that whatever that happened to be</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>I just like been tried to lose weight before and those things certainly have failed as I still I'm the same way</t>
+          <t>okay</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>,I've lost some pounds since starting off. So if anyone wants to try something else for themselves let them go ahead at their own pace whatever works best will work better than trying everything all over again which isn´t going anywhere anytime soon anyway</t>
+          <t>so you've done all these things in order to make yourself feel calmer, more relaxed, less anxious, and more comfortable?</t>
         </is>
       </c>
     </row>
@@ -903,17 +915,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>the golden retriever</t>
+          <t>it's good to see you again</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>oh nice</t>
+          <t>it's nice to see you</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>I'm sorry, did we just talk too long?</t>
+          <t>thank you for coming back to visit us</t>
         </is>
       </c>
     </row>
@@ -929,17 +941,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>all right so between now I'm going to see again do you have any hearings or anything coming up</t>
+          <t>okay tell me a little bit about how smoking fits in your day it'll help with the</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>no they're not for like a few more weeks</t>
+          <t>I mean I suppose a little less than a pack a day it's not too bad um the I probably smoked for the last five years but I I mean I could quit if I wanted to but I don't really want to right now</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>,I mean if something happens which would make us feel uncomfortable maybe next week. So basically as far back from here until after Christmas (laughs)</t>
+          <t>oh ok cool</t>
         </is>
       </c>
     </row>
@@ -955,17 +967,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>oh I would definitely say a ten</t>
+          <t>okay what made you say two instead of one</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>okay</t>
+          <t>well I mean anything's possible I mean I I guess I could maybe be convinced yeah is there something I mean I are there things I can try that would make me like want to quit smoking</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reflections : So let us start off today, first thing will probably help get rid or reduce stress. First step which might sound obvious because most people who go into recovery usually try to avoid any sort oof physical activity until after their illness has passed? What does exercising actually entail? Well basically once someone gets sick enough something happens inside them where everything starts changing. It changes our physiology,our brain chemistry change too cause every cell within each body part becomes different depending upon its function (or lack thereof) causing pain receptors around those areas become activated making muscles contract harder giving blood flow easier allowing oxygen to enter cells creating new tissue forming bones etc.. This process takes time though sometimes taking days maybe months before symptoms appear again The next important point regarding exercises itself isn tis very simple; Exercise helps keep energy levels high throughout the day while keeping hunger low during times of rest periods such being sleep deprivation periods When looking over many studies done since 2000 showing benefits associated wi fitness training programs including strength building workouts i</t>
+          <t>no, just stop smoking. You know, we all need help in our lives. We should never give up trying to live life as best as we can. It doesn't matter whether or not you succeed at doing this. If you fail then you failed. That's it. So quit smoking now. Quit smoking now. Stop smoking now.</t>
         </is>
       </c>
     </row>

</xml_diff>